<commit_message>
tested some new combination
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VS saves\TP5_ObjectConnecte\TP5_ObjectConnecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5601B6F5-12BF-4F27-87AB-8DD245A8CFEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA59178-FEC0-4FF7-9535-BDB44E1CBFD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7644" yWindow="2664" windowWidth="34560" windowHeight="18696" xr2:uid="{8079A9C0-E8F5-4663-80D5-DF92195297D0}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8079A9C0-E8F5-4663-80D5-DF92195297D0}"/>
   </bookViews>
   <sheets>
     <sheet name="CartPole-V0" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>julien vadeboncoeur</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{FB7F9A0B-88C0-4F76-9673-A351DF02AF76}">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{FB7F9A0B-88C0-4F76-9673-A351DF02AF76}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{7AF021AE-AADB-4C59-8466-880549DFE35E}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{7AF021AE-AADB-4C59-8466-880549DFE35E}">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,199 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{656E3A81-CB7A-49EC-AD24-6795727C9F38}">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{656E3A81-CB7A-49EC-AD24-6795727C9F38}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{4EF55363-C504-4BB5-9344-E276BB2C936F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{57929515-6A96-4E73-A82C-1C5B7A96B0B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{6BC53472-F4BA-4A70-AFAD-7EDB11149822}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{31906375-642F-426A-A1E3-1F8D0581EEE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{E0AE62CE-F4BC-4154-A27E-E35F044B7094}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{8CB19A32-DE89-4BEE-86C4-D088E843342E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{4500F594-BCF4-451E-952F-C0CCAB25024B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>julien vadeboncoeur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{953A905C-0EC9-4878-8607-89183D35C489}">
       <text>
         <r>
           <rPr>
@@ -106,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>Learning rate</t>
   </si>
@@ -154,13 +346,70 @@
   </si>
   <si>
     <t>Resultat de l'algo Q-learning  avec l'envrionnement Cartpole-V1</t>
+  </si>
+  <si>
+    <t>minimum assez bas</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>Resultat similaire au test précéedant mais le maximum est moins stable</t>
+  </si>
+  <si>
+    <t>minimum plus élevé</t>
+  </si>
+  <si>
+    <t>une certaine disparité entre chaque tentative</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.00015</t>
+  </si>
+  <si>
+    <t>not good</t>
+  </si>
+  <si>
+    <t>augmenter la periode d'exploration ne donne pas de très bon resultat</t>
+  </si>
+  <si>
+    <t>Learning rate decay</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.00022</t>
+  </si>
+  <si>
+    <t>raccourci la periode d'apprentissage et le nombre de section pour la rendre plus concentrée</t>
+  </si>
+  <si>
+    <t>ne prend pas beaucoup de cycle pour finir le jeu</t>
+  </si>
+  <si>
+    <t>minimum bas mais moyenne assez élevé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +444,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -222,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +501,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,10 +519,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -557,19 +818,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BCA1FC-DBE9-4BBD-8CA2-3F8F2F4FED39}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="77.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="11" max="11" width="89.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -579,17 +841,17 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -609,16 +871,19 @@
         <v>5</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -640,17 +905,20 @@
       <c r="G5" s="1">
         <v>20</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1">
         <v>8000</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -661,7 +929,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" s="1">
         <v>3400</v>
@@ -672,14 +940,20 @@
       <c r="G6" s="1">
         <v>20</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1">
         <v>8000</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -690,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1">
         <v>3400</v>
@@ -701,11 +975,310 @@
       <c r="G7" s="1">
         <v>20</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1">
         <v>8000</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6500</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6500</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="1">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="1">
+        <v>10</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="1">
+        <v>10</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8000</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started writting some notes
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VS saves\TP5_ObjectConnecte\TP5_ObjectConnecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA59178-FEC0-4FF7-9535-BDB44E1CBFD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228C0596-7B84-4EE5-8801-43FD51E27E05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8079A9C0-E8F5-4663-80D5-DF92195297D0}"/>
+    <workbookView xWindow="8244" yWindow="3384" windowWidth="29040" windowHeight="15840" xr2:uid="{8079A9C0-E8F5-4663-80D5-DF92195297D0}"/>
   </bookViews>
   <sheets>
     <sheet name="CartPole-V0" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>